<commit_message>
Added calculations/write for average surcharge rate
</commit_message>
<xml_diff>
--- a/Report Pack/report_pack_templ.xlsx
+++ b/Report Pack/report_pack_templ.xlsx
@@ -16,13 +16,13 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
+    <t>Card Payments</t>
+  </si>
+  <si>
     <t>Count of Approved Payments</t>
   </si>
   <si>
     <t>Value of Approved Payments</t>
-  </si>
-  <si>
-    <t>Number of Declined/Approved</t>
   </si>
   <si>
     <t>Average Surcharge Rate</t>
@@ -105,8 +105,10 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <color rgb="4372c5"/>
-      <sz val="14"/>
+      <b/>
+      <color theme="5"/>
+      <sz val="16"/>
+      <name val="Calibri (Body)"/>
     </font>
     <font>
       <color theme="1"/>
@@ -116,10 +118,8 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <b/>
-      <color theme="5"/>
-      <sz val="16"/>
-      <name val="Calibri (Body)"/>
+      <color rgb="4372c5"/>
+      <sz val="14"/>
     </font>
   </fonts>
   <fills count="2">
@@ -157,9 +157,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -558,344 +558,376 @@
         <v>44378</v>
       </c>
     </row>
-    <row r="6" ht="22" customHeight="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" ht="22" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6">
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+    </row>
+    <row r="7" ht="19" customHeight="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
         <v>10</v>
       </c>
-      <c r="G6">
+      <c r="G7">
         <v>15</v>
       </c>
-      <c r="H6">
+      <c r="H7">
         <v>15</v>
       </c>
-      <c r="I6">
+      <c r="I7">
         <v>10</v>
       </c>
-      <c r="J6">
+      <c r="J7">
         <v>16</v>
       </c>
-      <c r="K6">
+      <c r="K7">
         <v>15</v>
       </c>
-      <c r="L6">
+      <c r="L7">
         <v>8</v>
       </c>
-      <c r="M6">
+      <c r="M7">
         <v>19</v>
       </c>
-      <c r="N6">
+      <c r="N7">
         <v>11</v>
       </c>
     </row>
-    <row r="7" ht="19" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7">
+    <row r="8" ht="19" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
         <v>40165.376000000004</v>
       </c>
-      <c r="G7">
+      <c r="G8">
         <v>83351.40400000001</v>
       </c>
-      <c r="H7">
+      <c r="H8">
         <v>77477.077</v>
       </c>
-      <c r="I7">
+      <c r="I8">
         <v>63772.048</v>
       </c>
-      <c r="J7">
+      <c r="J8">
         <v>78229.64300000001</v>
       </c>
-      <c r="K7">
+      <c r="K8">
         <v>81307.26049999999</v>
       </c>
-      <c r="L7">
+      <c r="L8">
         <v>37565.5125</v>
       </c>
-      <c r="M7">
+      <c r="M8">
         <v>99061.0655</v>
       </c>
     </row>
-    <row r="8" ht="19" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+    <row r="9" ht="19" customHeight="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0.011</v>
+      </c>
+      <c r="G9">
+        <v>0.011666666666666669</v>
+      </c>
+      <c r="H9">
+        <v>0.010333333333333335</v>
+      </c>
+      <c r="I9">
+        <v>0.008499999999999999</v>
+      </c>
+      <c r="J9">
+        <v>0.011875</v>
+      </c>
+      <c r="K9">
+        <v>0.011333333333333332</v>
+      </c>
+      <c r="L9">
+        <v>0.013125</v>
+      </c>
+      <c r="M9">
+        <v>0.00973684210526316</v>
+      </c>
+      <c r="N9">
+        <v>0.012727272727272728</v>
+      </c>
+    </row>
+    <row r="10" ht="21" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+    </row>
+    <row r="11" ht="19" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+    </row>
+    <row r="12" ht="19" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-    </row>
-    <row r="9" ht="19" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-    </row>
-    <row r="10" ht="21" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-    </row>
-    <row r="11" ht="19" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-    </row>
-    <row r="12" ht="19" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
     </row>
     <row r="13" ht="19" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
     </row>
     <row r="14" ht="19" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
     </row>
     <row r="15" ht="21" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
     </row>
     <row r="16" ht="19" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
     </row>
     <row r="17" ht="19" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
     </row>
     <row r="18" ht="21" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
+      <c r="A18" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
     </row>
     <row r="19" ht="19" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
     </row>
     <row r="20" ht="19" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
     </row>
     <row r="21" ht="19" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
+      <c r="A21" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
     </row>
     <row r="22" ht="21" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
+      <c r="A22" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
     </row>
     <row r="23" ht="19" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
+      <c r="A23" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
-      <c r="H23" s="4"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
     </row>
     <row r="24" ht="19" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
+      <c r="A24" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="4"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
     </row>
     <row r="25" ht="21" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="5" t="s">
+      <c r="A25" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="4"/>
-      <c r="H25" s="4"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
     </row>
     <row r="26" ht="19" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
+      <c r="A26" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
-      <c r="H26" s="4"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
     </row>
     <row r="27" ht="19" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
+      <c r="A27" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
-      <c r="H27" s="4"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
     </row>
     <row r="28" ht="19" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
+      <c r="A28" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
-      <c r="H28" s="4"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Dates filled in programmatically
</commit_message>
<xml_diff>
--- a/Report Pack/report_pack_templ.xlsx
+++ b/Report Pack/report_pack_templ.xlsx
@@ -14,7 +14,46 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
+  <si>
+    <t>8-2022</t>
+  </si>
+  <si>
+    <t>7-2022</t>
+  </si>
+  <si>
+    <t>6-2022</t>
+  </si>
+  <si>
+    <t>5-2022</t>
+  </si>
+  <si>
+    <t>4-2022</t>
+  </si>
+  <si>
+    <t>3-2022</t>
+  </si>
+  <si>
+    <t>2-2022</t>
+  </si>
+  <si>
+    <t>13-2021</t>
+  </si>
+  <si>
+    <t>12-2021</t>
+  </si>
+  <si>
+    <t>11-2021</t>
+  </si>
+  <si>
+    <t>10-2021</t>
+  </si>
+  <si>
+    <t>9-2021</t>
+  </si>
+  <si>
+    <t>8-2021</t>
+  </si>
   <si>
     <t>Card Payments</t>
   </si>
@@ -95,13 +134,6 @@
       <family val="2"/>
       <scheme val="minor"/>
       <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <color theme="4"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-      <sz val="14"/>
       <name val="Calibri"/>
     </font>
     <font>
@@ -121,6 +153,13 @@
       <color rgb="4372c5"/>
       <sz val="14"/>
     </font>
+    <font>
+      <color theme="4"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+      <sz val="14"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -130,7 +169,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -138,28 +177,16 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thick">
-        <color theme="5"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="17" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -535,44 +562,62 @@
     <col min="2" max="2" width="16.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" ht="20" customHeight="1" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="1">
-        <v>44197</v>
-      </c>
-      <c r="C5" s="1">
-        <v>44228</v>
-      </c>
-      <c r="D5" s="1">
-        <v>44256</v>
-      </c>
-      <c r="E5" s="1">
-        <v>44287</v>
-      </c>
-      <c r="F5" s="1">
-        <v>44317</v>
-      </c>
-      <c r="G5" s="1">
-        <v>44348</v>
-      </c>
-      <c r="H5" s="1">
-        <v>44378</v>
+    <row r="5" ht="20" customHeight="1" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I5" t="s">
+        <v>7</v>
+      </c>
+      <c r="J5" t="s">
+        <v>8</v>
+      </c>
+      <c r="K5" t="s">
+        <v>9</v>
+      </c>
+      <c r="L5" t="s">
+        <v>10</v>
+      </c>
+      <c r="M5" t="s">
+        <v>11</v>
+      </c>
+      <c r="N5" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="6" ht="22" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
+      <c r="A6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
     </row>
     <row r="7" ht="19" customHeight="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>1</v>
+      <c r="A7" s="3" t="s">
+        <v>14</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -615,8 +660,8 @@
       </c>
     </row>
     <row r="8" ht="19" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>2</v>
+      <c r="A8" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -656,8 +701,8 @@
       </c>
     </row>
     <row r="9" ht="19" customHeight="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>3</v>
+      <c r="A9" s="3" t="s">
+        <v>16</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -700,234 +745,234 @@
       </c>
     </row>
     <row r="10" ht="21" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
+      <c r="A10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
     </row>
     <row r="11" ht="19" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
+      <c r="A11" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
     </row>
     <row r="12" ht="19" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
+      <c r="A12" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
     </row>
     <row r="13" ht="19" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
+      <c r="A13" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
     </row>
     <row r="14" ht="19" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
+      <c r="A14" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
     </row>
     <row r="15" ht="21" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
+      <c r="A15" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
     </row>
     <row r="16" ht="19" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
+      <c r="A16" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
     </row>
     <row r="17" ht="19" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
+      <c r="A17" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
     </row>
     <row r="18" ht="21" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
+      <c r="A18" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
     </row>
     <row r="19" ht="19" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
+      <c r="A19" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
     </row>
     <row r="20" ht="19" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
+      <c r="A20" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
     </row>
     <row r="21" ht="19" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
+      <c r="A21" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
     </row>
     <row r="22" ht="21" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
+      <c r="A22" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
     </row>
     <row r="23" ht="19" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
+      <c r="A23" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
     </row>
     <row r="24" ht="19" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-      <c r="H24" s="3"/>
+      <c r="A24" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
     </row>
     <row r="25" ht="21" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
-      <c r="H25" s="3"/>
+      <c r="A25" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
     </row>
     <row r="26" ht="19" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-      <c r="H26" s="3"/>
+      <c r="A26" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
     </row>
     <row r="27" ht="19" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
-      <c r="H27" s="3"/>
+      <c r="A27" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
     </row>
     <row r="28" ht="19" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
-      <c r="H28" s="3"/>
+      <c r="A28" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Calculation & Write of Approved Direct Debit Payment Values Complete
</commit_message>
<xml_diff>
--- a/Report Pack/report_pack_templ.xlsx
+++ b/Report Pack/report_pack_templ.xlsx
@@ -775,17 +775,49 @@
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
     </row>
-    <row r="12" ht="19" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
+    <row r="12" ht="19" customHeight="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>92390.01700000002</v>
+      </c>
+      <c r="G12">
+        <v>41463.556000000004</v>
+      </c>
+      <c r="H12">
+        <v>86566.3205</v>
+      </c>
+      <c r="I12">
+        <v>29267.3985</v>
+      </c>
+      <c r="J12">
+        <v>62031.90700000001</v>
+      </c>
+      <c r="K12">
+        <v>49470.471</v>
+      </c>
+      <c r="L12">
+        <v>36927.276</v>
+      </c>
+      <c r="M12">
+        <v>64959.96200000001</v>
+      </c>
+      <c r="N12">
+        <v>60838.859500000006</v>
+      </c>
     </row>
     <row r="13" ht="19" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">

</xml_diff>

<commit_message>
Added ExpressJS Package for Webserver + Significantly Reduced Code and Errors
</commit_message>
<xml_diff>
--- a/Report Pack/report_pack_templ.xlsx
+++ b/Report Pack/report_pack_templ.xlsx
@@ -14,7 +14,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
+  <si>
+    <t>Oct-2022</t>
+  </si>
   <si>
     <t>Sep-2022</t>
   </si>
@@ -52,9 +55,6 @@
     <t>Oct-2021</t>
   </si>
   <si>
-    <t>Sep-2021</t>
-  </si>
-  <si>
     <t>Card Payments</t>
   </si>
   <si>
@@ -68,9 +68,6 @@
   </si>
   <si>
     <t>Direct Debit Payments</t>
-  </si>
-  <si>
-    <t>Number of Approved Payments</t>
   </si>
   <si>
     <t>Dishonored Direct Debits</t>
@@ -639,31 +636,31 @@
         <v>0</v>
       </c>
       <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
         <v>10</v>
-      </c>
-      <c r="G7">
-        <v>15</v>
       </c>
       <c r="H7">
         <v>15</v>
       </c>
       <c r="I7">
+        <v>15</v>
+      </c>
+      <c r="J7">
         <v>10</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <v>16</v>
       </c>
-      <c r="K7">
+      <c r="L7">
         <v>15</v>
       </c>
-      <c r="L7">
+      <c r="M7">
         <v>8</v>
       </c>
-      <c r="M7">
+      <c r="N7">
         <v>19</v>
-      </c>
-      <c r="N7">
-        <v>11</v>
       </c>
     </row>
     <row r="8" ht="19" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -683,28 +680,28 @@
         <v>0</v>
       </c>
       <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
         <v>40165.376000000004</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>83351.40400000001</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>77477.077</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <v>63772.048</v>
       </c>
-      <c r="J8">
+      <c r="K8">
         <v>78229.64300000001</v>
       </c>
-      <c r="K8">
+      <c r="L8">
         <v>81307.26049999999</v>
       </c>
-      <c r="L8">
+      <c r="M8">
         <v>37565.5125</v>
-      </c>
-      <c r="M8">
-        <v>99061.0655</v>
       </c>
     </row>
     <row r="9" ht="19" customHeight="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -724,31 +721,31 @@
         <v>0</v>
       </c>
       <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
         <v>0.011</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>0.011666666666666669</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <v>0.010333333333333335</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <v>0.008499999999999999</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <v>0.011875</v>
       </c>
-      <c r="K9">
+      <c r="L9">
         <v>0.011333333333333332</v>
       </c>
-      <c r="L9">
+      <c r="M9">
         <v>0.013125</v>
       </c>
-      <c r="M9">
+      <c r="N9">
         <v>0.00973684210526316</v>
-      </c>
-      <c r="N9">
-        <v>0.012727272727272728</v>
       </c>
     </row>
     <row r="10" ht="21" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -763,17 +760,49 @@
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
     </row>
-    <row r="11" ht="19" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+    <row r="11" ht="19" customHeight="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
         <v>18</v>
       </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
+      <c r="H11">
+        <v>12</v>
+      </c>
+      <c r="I11">
+        <v>15</v>
+      </c>
+      <c r="J11">
+        <v>7</v>
+      </c>
+      <c r="K11">
+        <v>16</v>
+      </c>
+      <c r="L11">
+        <v>11</v>
+      </c>
+      <c r="M11">
+        <v>6</v>
+      </c>
+      <c r="N11">
+        <v>13</v>
+      </c>
     </row>
     <row r="12" ht="19" customHeight="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
@@ -792,36 +821,36 @@
         <v>0</v>
       </c>
       <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
         <v>92390.01700000002</v>
       </c>
-      <c r="G12">
+      <c r="H12">
         <v>41463.556000000004</v>
       </c>
-      <c r="H12">
+      <c r="I12">
         <v>86566.3205</v>
       </c>
-      <c r="I12">
+      <c r="J12">
         <v>29267.3985</v>
       </c>
-      <c r="J12">
+      <c r="K12">
         <v>62031.90700000001</v>
       </c>
-      <c r="K12">
+      <c r="L12">
         <v>49470.471</v>
       </c>
-      <c r="L12">
+      <c r="M12">
         <v>36927.276</v>
       </c>
-      <c r="M12">
+      <c r="N12">
         <v>64959.96200000001</v>
-      </c>
-      <c r="N12">
-        <v>60838.859500000006</v>
       </c>
     </row>
     <row r="13" ht="19" customHeight="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -836,36 +865,36 @@
         <v>0</v>
       </c>
       <c r="F13">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="G13">
         <v>13</v>
       </c>
       <c r="H13">
+        <v>13</v>
+      </c>
+      <c r="I13">
         <v>9</v>
       </c>
-      <c r="I13">
+      <c r="J13">
         <v>13</v>
       </c>
-      <c r="J13">
+      <c r="K13">
         <v>10</v>
       </c>
-      <c r="K13">
+      <c r="L13">
         <v>15</v>
       </c>
-      <c r="L13">
+      <c r="M13">
         <v>14</v>
       </c>
-      <c r="M13">
+      <c r="N13">
         <v>17</v>
-      </c>
-      <c r="N13">
-        <v>10</v>
       </c>
     </row>
     <row r="14" ht="19" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -877,7 +906,7 @@
     </row>
     <row r="15" ht="21" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -889,7 +918,7 @@
     </row>
     <row r="16" ht="19" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -901,7 +930,7 @@
     </row>
     <row r="17" ht="19" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -913,7 +942,7 @@
     </row>
     <row r="18" ht="21" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -925,10 +954,10 @@
     </row>
     <row r="19" ht="19" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>26</v>
       </c>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
@@ -939,7 +968,7 @@
     </row>
     <row r="20" ht="19" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -951,7 +980,7 @@
     </row>
     <row r="21" ht="19" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -963,7 +992,7 @@
     </row>
     <row r="22" ht="21" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -975,7 +1004,7 @@
     </row>
     <row r="23" ht="19" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -987,7 +1016,7 @@
     </row>
     <row r="24" ht="19" customHeight="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B24">
         <v>0</v>
@@ -1002,36 +1031,36 @@
         <v>0</v>
       </c>
       <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
         <v>105</v>
       </c>
-      <c r="G24">
+      <c r="H24">
         <v>81</v>
       </c>
-      <c r="H24">
+      <c r="I24">
         <v>89</v>
       </c>
-      <c r="I24">
+      <c r="J24">
         <v>72</v>
       </c>
-      <c r="J24">
+      <c r="K24">
         <v>96</v>
       </c>
-      <c r="K24">
+      <c r="L24">
         <v>71</v>
       </c>
-      <c r="L24">
+      <c r="M24">
         <v>72</v>
       </c>
-      <c r="M24">
+      <c r="N24">
         <v>101</v>
-      </c>
-      <c r="N24">
-        <v>93</v>
       </c>
     </row>
     <row r="25" ht="21" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -1043,7 +1072,7 @@
     </row>
     <row r="26" ht="19" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -1055,7 +1084,7 @@
     </row>
     <row r="27" ht="19" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -1067,7 +1096,7 @@
     </row>
     <row r="28" ht="19" customHeight="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>

</xml_diff>